<commit_message>
Ran analyses for full dataset, added some estimation across time. First draft of results
</commit_message>
<xml_diff>
--- a/Writing/Tables/Table2.xlsx
+++ b/Writing/Tables/Table2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Dropbox\CJM\Masterproject\Writing\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\SkyDrive\Masterproject\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>DP</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Journal</t>
   </si>
   <si>
-    <t>Significant</t>
-  </si>
-  <si>
-    <t>Nonsignificant</t>
-  </si>
-  <si>
     <t>Timeframe</t>
   </si>
   <si>
@@ -75,6 +69,33 @@
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>Acronym</t>
+  </si>
+  <si>
+    <t>Developmental Psychology</t>
+  </si>
+  <si>
+    <t>Frontiers in Psychology</t>
+  </si>
+  <si>
+    <t>Journal of Applied Psychology</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology: General</t>
+  </si>
+  <si>
+    <t>Journal of Personality and Social Psychology</t>
+  </si>
+  <si>
+    <t>Public Library of Science</t>
+  </si>
+  <si>
+    <t>Psychological Science</t>
+  </si>
+  <si>
+    <t>Journal of Consulting and Clinical Psychology</t>
   </si>
 </sst>
 </file>
@@ -132,11 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,191 +441,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E11"/>
+      <selection activeCell="C2" sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2782</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3519</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3381</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1184</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5108</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2307</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>36197</v>
-      </c>
-      <c r="D3" s="1">
-        <v>27909</v>
-      </c>
-      <c r="E3" s="1">
-        <v>8288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9712</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6904</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2808</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>14215</v>
-      </c>
-      <c r="D5" s="1">
-        <v>10582</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3633</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>26218</v>
-      </c>
-      <c r="D6" s="1">
-        <v>19632</v>
-      </c>
-      <c r="E6" s="1">
-        <v>6586</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>18733</v>
-      </c>
-      <c r="D7" s="1">
-        <v>13514</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>98061</v>
-      </c>
       <c r="D8" s="1">
-        <v>73644</v>
-      </c>
-      <c r="E8" s="1">
-        <v>24417</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>2126</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>10303</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1">
-        <v>29655</v>
-      </c>
-      <c r="D9" s="1">
-        <v>20289</v>
-      </c>
-      <c r="E9" s="1">
-        <v>9366</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1">
-        <v>15092</v>
-      </c>
-      <c r="D10" s="1">
-        <v>11655</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3">
-        <f>SUM(C3:C10)</f>
-        <v>247883</v>
-      </c>
-      <c r="D11" s="3">
-        <f>SUM(D3:D10)</f>
-        <v>184129</v>
-      </c>
-      <c r="E11" s="3">
-        <f>SUM(E3:E10)</f>
-        <v>63754</v>
-      </c>
+      <c r="D10" s="3">
+        <v>30710</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrected error in simNullDist.R, wrote
</commit_message>
<xml_diff>
--- a/Writing/Tables/Table2.xlsx
+++ b/Writing/Tables/Table2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Timeframe</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Psychological Science (PS)</t>
+  </si>
+  <si>
+    <t>Check</t>
   </si>
 </sst>
 </file>
@@ -125,12 +128,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -165,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -217,6 +226,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -516,9 +536,10 @@
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -546,8 +567,12 @@
       <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J1" s="22"/>
+      <c r="K1" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -564,21 +589,26 @@
         <v>13.54358</v>
       </c>
       <c r="F2" s="3">
-        <v>18032</v>
+        <v>24584</v>
       </c>
       <c r="G2" s="13">
         <f>F2/D2</f>
-        <v>0.58318240620957307</v>
+        <v>0.79508408796895214</v>
       </c>
       <c r="H2" s="3">
-        <v>12888</v>
+        <v>6336</v>
       </c>
       <c r="I2" s="13">
         <f>H2/D2</f>
-        <v>0.41681759379042693</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.20491591203104786</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="20">
+        <f>F2+H2</f>
+        <v>30920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -595,21 +625,26 @@
         <v>14.93811</v>
       </c>
       <c r="F3" s="3">
-        <v>4655</v>
+        <v>6595</v>
       </c>
       <c r="G3" s="13">
         <f t="shared" ref="G3:G9" si="0">F3/D3</f>
-        <v>0.50752289576973397</v>
+        <v>0.71903619712167466</v>
       </c>
       <c r="H3" s="3">
-        <v>4517</v>
+        <v>2577</v>
       </c>
       <c r="I3" s="13">
         <f t="shared" ref="I3:I9" si="1">H3/D3</f>
-        <v>0.49247710423026603</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.28096380287832534</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="20">
+        <f t="shared" ref="K3:K10" si="2">F3+H3</f>
+        <v>9172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -626,21 +661,26 @@
         <v>9.0718320000000006</v>
       </c>
       <c r="F4" s="3">
-        <v>5926</v>
+        <v>8455</v>
       </c>
       <c r="G4" s="13">
         <f t="shared" si="0"/>
-        <v>0.52722419928825626</v>
+        <v>0.75222419928825623</v>
       </c>
       <c r="H4" s="3">
-        <v>5314</v>
+        <v>2785</v>
       </c>
       <c r="I4" s="13">
         <f t="shared" si="1"/>
-        <v>0.4727758007117438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.24777580071174377</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="20">
+        <f t="shared" si="2"/>
+        <v>11240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -657,21 +697,26 @@
         <v>9.8494360000000007</v>
       </c>
       <c r="F5" s="3">
-        <v>11770</v>
+        <v>15672</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="0"/>
-        <v>0.58606781855300505</v>
+        <v>0.78036149977592995</v>
       </c>
       <c r="H5" s="3">
-        <v>8313</v>
+        <v>4411</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" si="1"/>
-        <v>0.41393218144699495</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.21963850022407011</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="20">
+        <f t="shared" si="2"/>
+        <v>20083</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -688,21 +733,26 @@
         <v>22.387309999999999</v>
       </c>
       <c r="F6" s="3">
-        <v>8980</v>
+        <v>12706</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="0"/>
-        <v>0.51958572007174675</v>
+        <v>0.73517329167389922</v>
       </c>
       <c r="H6" s="3">
-        <v>8303</v>
+        <v>4577</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="1"/>
-        <v>0.4804142799282532</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.26482670832610078</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="20">
+        <f t="shared" si="2"/>
+        <v>17283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -719,21 +769,26 @@
         <v>22.45926</v>
       </c>
       <c r="F7" s="3">
-        <v>52796</v>
+        <v>69836</v>
       </c>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
-        <v>0.57517621553311327</v>
+        <v>0.76081533047902294</v>
       </c>
       <c r="H7" s="3">
-        <v>38995</v>
+        <v>21955</v>
       </c>
       <c r="I7" s="13">
         <f t="shared" si="1"/>
-        <v>0.42482378446688673</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.239184669520977</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="20">
+        <f t="shared" si="2"/>
+        <v>91791</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -750,21 +805,26 @@
         <v>13.186059999999999</v>
       </c>
       <c r="F8" s="3">
-        <v>14431</v>
+        <v>19696</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
-        <v>0.50526942333951896</v>
+        <v>0.68961170827351981</v>
       </c>
       <c r="H8" s="3">
-        <v>14130</v>
+        <v>8865</v>
       </c>
       <c r="I8" s="13">
         <f t="shared" si="1"/>
-        <v>0.49473057666048109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.31038829172648019</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="20">
+        <f t="shared" si="2"/>
+        <v>28561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -781,21 +841,26 @@
         <v>8.9661340000000003</v>
       </c>
       <c r="F9" s="7">
-        <v>8358</v>
+        <v>10943</v>
       </c>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
-        <v>0.59563854047890541</v>
+        <v>0.77986031927023947</v>
       </c>
       <c r="H9" s="7">
-        <v>5674</v>
+        <v>3089</v>
       </c>
       <c r="I9" s="13">
         <f t="shared" si="1"/>
-        <v>0.40436145952109465</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>0.22013968072976053</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="20">
+        <f t="shared" si="2"/>
+        <v>14032</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
         <v>8</v>
@@ -813,24 +878,30 @@
       </c>
       <c r="F10" s="11">
         <f>SUM(F2:F9)</f>
-        <v>124948</v>
+        <v>168487</v>
       </c>
       <c r="G10" s="12">
         <f>F10/D10</f>
-        <v>0.56009897705776346</v>
+        <v>0.75526936283519064</v>
       </c>
       <c r="H10" s="11">
         <f>SUM(H2:H9)</f>
-        <v>98134</v>
+        <v>54595</v>
       </c>
       <c r="I10" s="12">
         <f>H10/D10</f>
-        <v>0.43990102294223649</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.24473063716480936</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="20">
+        <f t="shared" si="2"/>
+        <v>223082</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="17"/>
       <c r="F11" s="18"/>
+      <c r="K11" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>